<commit_message>
Updated solution models EF21
added clinohumite, pyrrhotite
</commit_message>
<xml_diff>
--- a/Solutions/solution_models_EF21.xlsx
+++ b/Solutions/solution_models_EF21.xlsx
@@ -5,25 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Thermolab\Github\Solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Thermolab\v_23_10_09\Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFAEAB0-C2F7-4294-9D28-58B7FC7D9678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA4C05B-EC98-4109-B6BE-A6D68319042D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="1650" windowWidth="23655" windowHeight="15480" activeTab="3" xr2:uid="{EF84C4B9-D779-4E3F-B62A-26420BF8ED2A}"/>
+    <workbookView xWindow="5550" yWindow="2775" windowWidth="23655" windowHeight="15480" activeTab="4" xr2:uid="{EF84C4B9-D779-4E3F-B62A-26420BF8ED2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fluid" sheetId="11" r:id="rId1"/>
     <sheet name="Olivine" sheetId="2" r:id="rId2"/>
     <sheet name="Antigorite" sheetId="3" r:id="rId3"/>
-    <sheet name="Brucite (2)" sheetId="13" r:id="rId4"/>
-    <sheet name="Brucite" sheetId="4" r:id="rId5"/>
-    <sheet name="Talc" sheetId="5" r:id="rId6"/>
-    <sheet name="Orthopyroxene" sheetId="6" r:id="rId7"/>
-    <sheet name="Chlorite" sheetId="7" r:id="rId8"/>
-    <sheet name="Garnet" sheetId="8" r:id="rId9"/>
-    <sheet name="Spinel" sheetId="10" r:id="rId10"/>
-    <sheet name="Lizardite" sheetId="12" r:id="rId11"/>
+    <sheet name="Brucite" sheetId="4" r:id="rId4"/>
+    <sheet name="Clinohumite" sheetId="15" r:id="rId5"/>
+    <sheet name="Pyrrhotite" sheetId="14" r:id="rId6"/>
+    <sheet name="Talc" sheetId="5" r:id="rId7"/>
+    <sheet name="Orthopyroxene" sheetId="6" r:id="rId8"/>
+    <sheet name="Chlorite" sheetId="7" r:id="rId9"/>
+    <sheet name="Garnet" sheetId="8" r:id="rId10"/>
+    <sheet name="Spinel" sheetId="10" r:id="rId11"/>
+    <sheet name="Lizardite" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="107">
   <si>
     <t>Modeltype</t>
   </si>
@@ -343,10 +344,28 @@
     <t>fliz,tc-ds633</t>
   </si>
   <si>
-    <t>M0</t>
-  </si>
-  <si>
-    <t>fbr,tc-ds633</t>
+    <t>trov,tc-ds633</t>
+  </si>
+  <si>
+    <t>trot,tc-ds633</t>
+  </si>
+  <si>
+    <t>trov</t>
+  </si>
+  <si>
+    <t>trot</t>
+  </si>
+  <si>
+    <t>chum,tc-ds633</t>
+  </si>
+  <si>
+    <t>chuf,tc-ds633</t>
+  </si>
+  <si>
+    <t>chum</t>
+  </si>
+  <si>
+    <t>chuf</t>
   </si>
 </sst>
 </file>
@@ -704,7 +723,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,6 +843,241 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE0E4CC-BF23-4D97-B5ED-C14DA256414F}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="C13">
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>4000</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="3">
+        <v>4000</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>100</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="3">
+        <v>100</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034B7D30-79D8-4EE2-AA72-AAF4766A8FCE}">
   <dimension ref="A1:E20"/>
   <sheetViews>
@@ -1072,12 +1326,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4D5436-75BD-41AA-AB99-0A6FE4652DF2}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1453,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C31"/>
+      <selection activeCell="A16" sqref="A16:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1989,128 +2243,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C24A454-5D99-4B41-9830-B9433EF0A31A}">
-  <dimension ref="A1:C14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="C13">
-        <v>6.7000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7A5922-32A1-4525-A8D5-08291F88DE91}">
   <dimension ref="A1:C26"/>
   <sheetViews>
@@ -2257,7 +2389,337 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB84638-00A4-49FD-BD1E-26BAF827F71F}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13" si="0">1/15</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="2">
+        <v>36000</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B632DE35-A95A-473D-A331-529862D5663F}">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13" si="0">1/15</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-3190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="2">
+        <v>-3190</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11195E3F-6D4E-40FF-8E1F-830C43F1246E}">
   <dimension ref="A1:J26"/>
   <sheetViews>
@@ -2866,7 +3328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664EBA9F-485E-4D12-9274-D8DC2566B140}">
   <dimension ref="A1:I38"/>
   <sheetViews>
@@ -3610,7 +4072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9786E4BD-A981-45AF-BC58-5212707790B9}">
   <dimension ref="A1:N30"/>
   <sheetViews>
@@ -4568,239 +5030,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE0E4CC-BF23-4D97-B5ED-C14DA256414F}">
-  <dimension ref="A1:E26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <f>1/15</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="C13">
-        <f>1/15</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3">
-        <v>4000</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="3">
-        <v>4000</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="3">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="3">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3">
-        <v>100</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="3">
-        <v>100</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>